<commit_message>
More work on the date parsng
</commit_message>
<xml_diff>
--- a/backend/app/Console/Commands/example_files/dummy_file.xlsx
+++ b/backend/app/Console/Commands/example_files/dummy_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/financeular/backend/src/file/example_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/financeular/backend/app/Console/Commands/example_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843D33C3-545C-0843-B2D0-47966858985F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FA1653-9A1C-3647-8A83-BB6EF0BE8570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20980" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="דצמבר 2019" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="275">
   <si>
     <t>כמה נכנס כסף בפועל</t>
   </si>
@@ -488,9 +488,6 @@
   </si>
   <si>
     <t>בריתות</t>
-  </si>
-  <si>
-    <t>גלידה</t>
   </si>
   <si>
     <t>אוכל בעבודה</t>
@@ -876,7 +873,7 @@
     <numFmt numFmtId="164" formatCode="[$ ₪]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="mm/dd"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -923,6 +920,10 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Nunito"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2704,10 +2705,10 @@
   <dimension ref="A1:U62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="L10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="T55" sqref="T55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3948,7 +3949,9 @@
       <c r="R58" s="22">
         <v>430</v>
       </c>
-      <c r="S58" s="29"/>
+      <c r="S58" s="35" t="s">
+        <v>134</v>
+      </c>
       <c r="T58" s="24" t="s">
         <v>135</v>
       </c>
@@ -3979,6 +3982,7 @@
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="R2:T2"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3988,13 +3992,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U62"/>
+  <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -4253,7 +4257,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="27">
-        <f>SUM(R4:R1004)</f>
+        <f>SUM(R4:R1003)</f>
         <v>10148</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -4934,28 +4938,30 @@
       <c r="R32" s="22">
         <v>600</v>
       </c>
-      <c r="S32" s="23"/>
+      <c r="S32" s="35" t="s">
+        <v>147</v>
+      </c>
       <c r="T32" s="24" t="s">
         <v>149</v>
       </c>
       <c r="U32" s="25"/>
     </row>
     <row r="33" spans="18:21" ht="18">
-      <c r="R33" s="22"/>
-      <c r="S33" s="23"/>
+      <c r="R33" s="22">
+        <v>500</v>
+      </c>
+      <c r="S33" s="35" t="s">
+        <v>147</v>
+      </c>
       <c r="T33" s="24" t="s">
         <v>150</v>
       </c>
       <c r="U33" s="25"/>
     </row>
     <row r="34" spans="18:21" ht="18">
-      <c r="R34" s="22">
-        <v>500</v>
-      </c>
+      <c r="R34" s="22"/>
       <c r="S34" s="29"/>
-      <c r="T34" s="24" t="s">
-        <v>151</v>
-      </c>
+      <c r="T34" s="24"/>
       <c r="U34" s="25"/>
     </row>
     <row r="35" spans="18:21" ht="18">
@@ -5004,7 +5010,6 @@
       <c r="R42" s="22"/>
       <c r="S42" s="29"/>
       <c r="T42" s="24"/>
-      <c r="U42" s="25"/>
     </row>
     <row r="43" spans="18:21" ht="18">
       <c r="R43" s="22"/>
@@ -5100,11 +5105,6 @@
       <c r="R61" s="22"/>
       <c r="S61" s="29"/>
       <c r="T61" s="24"/>
-    </row>
-    <row r="62" spans="18:20" ht="18">
-      <c r="R62" s="22"/>
-      <c r="S62" s="29"/>
-      <c r="T62" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5307,7 +5307,7 @@
         <v>500</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="16">
@@ -5460,7 +5460,7 @@
         <v>43893</v>
       </c>
       <c r="T8" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U8" s="25"/>
     </row>
@@ -5505,7 +5505,7 @@
         <v>43894</v>
       </c>
       <c r="T9" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -5623,7 +5623,7 @@
         <v>43924</v>
       </c>
       <c r="T12" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U12" s="25"/>
     </row>
@@ -5730,7 +5730,7 @@
         <v>43985</v>
       </c>
       <c r="T16" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U16" s="25"/>
     </row>
@@ -5754,7 +5754,7 @@
         <v>43985</v>
       </c>
       <c r="T17" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U17" s="25"/>
     </row>
@@ -5778,7 +5778,7 @@
         <v>43985</v>
       </c>
       <c r="T18" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U18" s="25"/>
     </row>
@@ -5802,7 +5802,7 @@
         <v>43985</v>
       </c>
       <c r="T19" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="U19" s="25"/>
     </row>
@@ -5826,7 +5826,7 @@
         <v>43985</v>
       </c>
       <c r="T20" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="U20" s="25"/>
     </row>
@@ -5847,7 +5847,7 @@
         <v>43985</v>
       </c>
       <c r="T21" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U21" s="25"/>
     </row>
@@ -5889,7 +5889,7 @@
         <v>44046</v>
       </c>
       <c r="T23" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U23" s="25"/>
     </row>
@@ -5910,7 +5910,7 @@
         <v>44046</v>
       </c>
       <c r="T24" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U24" s="25"/>
     </row>
@@ -5994,7 +5994,7 @@
         <v>44138</v>
       </c>
       <c r="T28" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U28" s="25"/>
     </row>
@@ -6056,10 +6056,10 @@
         <v>114</v>
       </c>
       <c r="S31" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="T31" s="31" t="s">
         <v>165</v>
-      </c>
-      <c r="T31" s="31" t="s">
-        <v>166</v>
       </c>
       <c r="U31" s="25"/>
     </row>
@@ -6068,7 +6068,7 @@
         <v>210</v>
       </c>
       <c r="S32" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T32" s="24" t="s">
         <v>59</v>
@@ -6083,7 +6083,7 @@
         <v>44138</v>
       </c>
       <c r="T33" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U33" s="25"/>
     </row>
@@ -6092,7 +6092,7 @@
         <v>303</v>
       </c>
       <c r="S34" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T34" s="24" t="s">
         <v>83</v>
@@ -6104,7 +6104,7 @@
         <v>47</v>
       </c>
       <c r="S35" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T35" s="24" t="s">
         <v>70</v>
@@ -6116,7 +6116,7 @@
         <v>36</v>
       </c>
       <c r="S36" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T36" s="24" t="s">
         <v>70</v>
@@ -6128,10 +6128,10 @@
         <v>70.599999999999994</v>
       </c>
       <c r="S37" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="T37" s="24" t="s">
         <v>169</v>
-      </c>
-      <c r="T37" s="24" t="s">
-        <v>170</v>
       </c>
       <c r="U37" s="25"/>
     </row>
@@ -6140,7 +6140,7 @@
         <v>100</v>
       </c>
       <c r="S38" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T38" s="24" t="s">
         <v>95</v>
@@ -6152,7 +6152,7 @@
         <v>96</v>
       </c>
       <c r="S39" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T39" s="24" t="s">
         <v>70</v>
@@ -6164,7 +6164,7 @@
         <v>15</v>
       </c>
       <c r="S40" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T40" s="24" t="s">
         <v>73</v>
@@ -6176,7 +6176,7 @@
         <v>366</v>
       </c>
       <c r="S41" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T41" s="24" t="s">
         <v>61</v>
@@ -6188,10 +6188,10 @@
         <v>78</v>
       </c>
       <c r="S42" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="T42" s="24" t="s">
         <v>172</v>
-      </c>
-      <c r="T42" s="24" t="s">
-        <v>173</v>
       </c>
       <c r="U42" s="25"/>
     </row>
@@ -6200,7 +6200,7 @@
         <v>33</v>
       </c>
       <c r="S43" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T43" s="24" t="s">
         <v>57</v>
@@ -6211,10 +6211,10 @@
         <v>447</v>
       </c>
       <c r="S44" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="T44" s="24" t="s">
         <v>174</v>
-      </c>
-      <c r="T44" s="24" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="45" spans="18:21" ht="18">
@@ -6222,10 +6222,10 @@
         <v>85</v>
       </c>
       <c r="S45" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T45" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="18:21" ht="18">
@@ -6233,7 +6233,7 @@
         <v>75</v>
       </c>
       <c r="S46" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T46" s="24" t="s">
         <v>72</v>
@@ -6244,7 +6244,7 @@
         <v>73</v>
       </c>
       <c r="S47" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T47" s="24" t="s">
         <v>70</v>
@@ -6255,7 +6255,7 @@
         <v>22</v>
       </c>
       <c r="S48" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T48" s="24" t="s">
         <v>70</v>
@@ -6266,10 +6266,10 @@
         <v>72</v>
       </c>
       <c r="S49" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="T49" s="24" t="s">
         <v>178</v>
-      </c>
-      <c r="T49" s="24" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="50" spans="18:20" ht="18">
@@ -6277,10 +6277,10 @@
         <v>153</v>
       </c>
       <c r="S50" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="T50" s="24" t="s">
         <v>180</v>
-      </c>
-      <c r="T50" s="24" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="51" spans="18:20" ht="18">
@@ -6288,7 +6288,7 @@
         <v>86</v>
       </c>
       <c r="S51" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T51" s="24" t="s">
         <v>101</v>
@@ -6299,7 +6299,7 @@
         <v>97</v>
       </c>
       <c r="S52" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T52" s="24" t="s">
         <v>70</v>
@@ -6310,10 +6310,10 @@
         <v>100</v>
       </c>
       <c r="S53" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="T53" s="24" t="s">
         <v>183</v>
-      </c>
-      <c r="T53" s="24" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="54" spans="18:20" ht="18">
@@ -6321,7 +6321,7 @@
         <v>336</v>
       </c>
       <c r="S54" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T54" s="24" t="s">
         <v>61</v>
@@ -6332,10 +6332,10 @@
         <v>130</v>
       </c>
       <c r="S55" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="T55" s="24" t="s">
         <v>185</v>
-      </c>
-      <c r="T55" s="24" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="56" spans="18:20" ht="18">
@@ -6343,10 +6343,10 @@
         <v>180</v>
       </c>
       <c r="S56" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T56" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="18:20" ht="18">
@@ -6354,7 +6354,7 @@
         <v>72</v>
       </c>
       <c r="S57" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T57" s="24" t="s">
         <v>70</v>
@@ -6365,10 +6365,10 @@
         <v>84</v>
       </c>
       <c r="S58" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T58" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="18:20" ht="18">
@@ -6376,7 +6376,7 @@
         <v>73</v>
       </c>
       <c r="S59" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T59" s="24" t="s">
         <v>70</v>
@@ -6387,7 +6387,7 @@
         <v>71</v>
       </c>
       <c r="S60" s="29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T60" s="24" t="s">
         <v>84</v>
@@ -6398,7 +6398,7 @@
         <v>133</v>
       </c>
       <c r="S61" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T61" s="24" t="s">
         <v>84</v>
@@ -6409,7 +6409,7 @@
         <v>379</v>
       </c>
       <c r="S62" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T62" s="24" t="s">
         <v>131</v>
@@ -6616,7 +6616,7 @@
         <v>500</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="16">
@@ -6769,7 +6769,7 @@
         <v>43834</v>
       </c>
       <c r="T8" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U8" s="25"/>
     </row>
@@ -6814,7 +6814,7 @@
         <v>43834</v>
       </c>
       <c r="T9" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -7039,7 +7039,7 @@
         <v>43955</v>
       </c>
       <c r="T16" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U16" s="25"/>
     </row>
@@ -7258,7 +7258,7 @@
         <v>75</v>
       </c>
       <c r="S26" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T26" s="34" t="s">
         <v>72</v>
@@ -7279,7 +7279,7 @@
         <v>138</v>
       </c>
       <c r="S27" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T27" s="34" t="s">
         <v>84</v>
@@ -7300,7 +7300,7 @@
         <v>176</v>
       </c>
       <c r="S28" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="T28" s="34" t="s">
         <v>101</v>
@@ -7321,7 +7321,7 @@
         <v>103</v>
       </c>
       <c r="S29" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T29" s="34" t="s">
         <v>67</v>
@@ -7342,7 +7342,7 @@
         <v>20</v>
       </c>
       <c r="S30" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T30" s="34" t="s">
         <v>73</v>
@@ -7365,7 +7365,7 @@
         <v>65</v>
       </c>
       <c r="S31" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T31" s="34" t="s">
         <v>70</v>
@@ -7377,7 +7377,7 @@
         <v>272</v>
       </c>
       <c r="S32" s="35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T32" s="34" t="s">
         <v>83</v>
@@ -7389,7 +7389,7 @@
         <v>216</v>
       </c>
       <c r="S33" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T33" s="34" t="s">
         <v>59</v>
@@ -7401,7 +7401,7 @@
         <v>103</v>
       </c>
       <c r="S34" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T34" s="34" t="s">
         <v>59</v>
@@ -7413,10 +7413,10 @@
         <v>103</v>
       </c>
       <c r="S35" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T35" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U35" s="25"/>
     </row>
@@ -7425,10 +7425,10 @@
         <v>180</v>
       </c>
       <c r="S36" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="T36" s="34" t="s">
         <v>197</v>
-      </c>
-      <c r="T36" s="34" t="s">
-        <v>198</v>
       </c>
       <c r="U36" s="25"/>
     </row>
@@ -7437,7 +7437,7 @@
         <v>222</v>
       </c>
       <c r="S37" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T37" s="34" t="s">
         <v>84</v>
@@ -7449,7 +7449,7 @@
         <v>96</v>
       </c>
       <c r="S38" s="35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T38" s="34" t="s">
         <v>70</v>
@@ -7461,7 +7461,7 @@
         <v>340</v>
       </c>
       <c r="S39" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T39" s="34" t="s">
         <v>61</v>
@@ -7473,7 +7473,7 @@
         <v>215</v>
       </c>
       <c r="S40" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T40" s="34" t="s">
         <v>84</v>
@@ -7793,7 +7793,7 @@
         <v>2000</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="16">
@@ -7946,7 +7946,7 @@
         <v>43835</v>
       </c>
       <c r="T8" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U8" s="25"/>
     </row>
@@ -8240,7 +8240,7 @@
         <v>44017</v>
       </c>
       <c r="T17" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U17" s="25"/>
     </row>
@@ -8372,7 +8372,7 @@
         <v>36</v>
       </c>
       <c r="S23" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T23" s="24" t="s">
         <v>73</v>
@@ -8393,7 +8393,7 @@
         <v>23</v>
       </c>
       <c r="S24" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T24" s="24" t="s">
         <v>70</v>
@@ -8414,10 +8414,10 @@
         <v>75</v>
       </c>
       <c r="S25" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="T25" s="24" t="s">
         <v>203</v>
-      </c>
-      <c r="T25" s="24" t="s">
-        <v>204</v>
       </c>
       <c r="U25" s="25"/>
     </row>
@@ -8435,7 +8435,7 @@
         <v>135</v>
       </c>
       <c r="S26" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="T26" s="24" t="s">
         <v>55</v>
@@ -8456,7 +8456,7 @@
         <v>256</v>
       </c>
       <c r="S27" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="T27" s="24" t="s">
         <v>83</v>
@@ -8477,7 +8477,7 @@
         <v>50</v>
       </c>
       <c r="S28" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T28" s="24" t="s">
         <v>70</v>
@@ -8498,7 +8498,7 @@
         <v>36</v>
       </c>
       <c r="S29" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T29" s="24" t="s">
         <v>73</v>
@@ -8519,10 +8519,10 @@
         <v>90</v>
       </c>
       <c r="S30" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T30" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U30" s="25"/>
     </row>
@@ -8542,7 +8542,7 @@
         <v>291</v>
       </c>
       <c r="S31" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T31" s="31" t="s">
         <v>61</v>
@@ -8554,7 +8554,7 @@
         <v>40</v>
       </c>
       <c r="S32" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="T32" s="24" t="s">
         <v>70</v>
@@ -8566,10 +8566,10 @@
         <v>280</v>
       </c>
       <c r="S33" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="T33" s="31" t="s">
         <v>208</v>
-      </c>
-      <c r="T33" s="31" t="s">
-        <v>209</v>
       </c>
       <c r="U33" s="25"/>
     </row>
@@ -8578,7 +8578,7 @@
         <v>118</v>
       </c>
       <c r="S34" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T34" s="24" t="s">
         <v>84</v>
@@ -8590,7 +8590,7 @@
         <v>146</v>
       </c>
       <c r="S35" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T35" s="24" t="s">
         <v>70</v>
@@ -8602,7 +8602,7 @@
         <v>40</v>
       </c>
       <c r="S36" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T36" s="24" t="s">
         <v>84</v>
@@ -8614,10 +8614,10 @@
         <v>115</v>
       </c>
       <c r="S37" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T37" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U37" s="25"/>
     </row>
@@ -8626,7 +8626,7 @@
         <v>276</v>
       </c>
       <c r="S38" s="29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T38" s="24" t="s">
         <v>61</v>
@@ -8638,7 +8638,7 @@
         <v>56</v>
       </c>
       <c r="S39" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T39" s="24" t="s">
         <v>84</v>
@@ -8650,7 +8650,7 @@
         <v>290</v>
       </c>
       <c r="S40" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="T40" s="24" t="s">
         <v>59</v>
@@ -8662,10 +8662,10 @@
         <v>70</v>
       </c>
       <c r="S41" s="29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="T41" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U41" s="25"/>
     </row>
@@ -8674,7 +8674,7 @@
         <v>34</v>
       </c>
       <c r="S42" s="29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="T42" s="24" t="s">
         <v>70</v>
@@ -8686,10 +8686,10 @@
         <v>62</v>
       </c>
       <c r="S43" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="T43" s="24" t="s">
         <v>215</v>
-      </c>
-      <c r="T43" s="24" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="44" spans="18:21" ht="18">
@@ -8697,10 +8697,10 @@
         <v>28</v>
       </c>
       <c r="S44" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T44" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="18:21" ht="18">
@@ -8708,7 +8708,7 @@
         <v>52</v>
       </c>
       <c r="S45" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T45" s="24" t="s">
         <v>83</v>
@@ -8719,10 +8719,10 @@
         <v>235</v>
       </c>
       <c r="S46" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="T46" s="24" t="s">
         <v>218</v>
-      </c>
-      <c r="T46" s="24" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="47" spans="18:21" ht="18">
@@ -8730,7 +8730,7 @@
         <v>117</v>
       </c>
       <c r="S47" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T47" s="24" t="s">
         <v>85</v>
@@ -8741,10 +8741,10 @@
         <v>60</v>
       </c>
       <c r="S48" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T48" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="18:20" ht="18">
@@ -8752,10 +8752,10 @@
         <v>136</v>
       </c>
       <c r="S49" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="T49" s="24" t="s">
         <v>221</v>
-      </c>
-      <c r="T49" s="24" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="50" spans="18:20" ht="18">
@@ -8763,7 +8763,7 @@
         <v>395</v>
       </c>
       <c r="S50" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T50" s="24" t="s">
         <v>131</v>
@@ -9096,7 +9096,7 @@
         <v>43836</v>
       </c>
       <c r="T6" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U6" s="25"/>
     </row>
@@ -9143,7 +9143,7 @@
         <v>43836</v>
       </c>
       <c r="T7" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U7" s="25"/>
     </row>
@@ -9224,7 +9224,7 @@
         <v>43836</v>
       </c>
       <c r="T9" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -9260,7 +9260,7 @@
         <v>43836</v>
       </c>
       <c r="T10" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U10" s="25"/>
     </row>
@@ -9342,7 +9342,7 @@
         <v>44049</v>
       </c>
       <c r="T12" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U12" s="25"/>
     </row>
@@ -9401,7 +9401,7 @@
         <v>44080</v>
       </c>
       <c r="T14" s="24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U14" s="25"/>
     </row>
@@ -9494,7 +9494,7 @@
         <v>390</v>
       </c>
       <c r="S18" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="T18" s="24" t="s">
         <v>61</v>
@@ -9542,7 +9542,7 @@
         <v>110</v>
       </c>
       <c r="S20" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="T20" s="24" t="s">
         <v>95</v>
@@ -9563,7 +9563,7 @@
         <v>72</v>
       </c>
       <c r="S21" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T21" s="24" t="s">
         <v>70</v>
@@ -9584,7 +9584,7 @@
         <v>96</v>
       </c>
       <c r="S22" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T22" s="24" t="s">
         <v>84</v>
@@ -9605,10 +9605,10 @@
         <v>100</v>
       </c>
       <c r="S23" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T23" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U23" s="25"/>
     </row>
@@ -9626,7 +9626,7 @@
         <v>406</v>
       </c>
       <c r="S24" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T24" s="24" t="s">
         <v>61</v>
@@ -9647,7 +9647,7 @@
         <v>132</v>
       </c>
       <c r="S25" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T25" s="24" t="s">
         <v>84</v>
@@ -9668,7 +9668,7 @@
         <v>22</v>
       </c>
       <c r="S26" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T26" s="24" t="s">
         <v>70</v>
@@ -9689,10 +9689,10 @@
         <v>65</v>
       </c>
       <c r="S27" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T27" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U27" s="25"/>
     </row>
@@ -9710,10 +9710,10 @@
         <v>160</v>
       </c>
       <c r="S28" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="T28" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U28" s="25"/>
     </row>
@@ -9731,10 +9731,10 @@
         <v>36</v>
       </c>
       <c r="S29" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="T29" s="24" t="s">
         <v>229</v>
-      </c>
-      <c r="T29" s="24" t="s">
-        <v>230</v>
       </c>
       <c r="U29" s="25"/>
     </row>
@@ -9752,10 +9752,10 @@
         <v>90</v>
       </c>
       <c r="S30" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="T30" s="31" t="s">
         <v>231</v>
-      </c>
-      <c r="T30" s="31" t="s">
-        <v>232</v>
       </c>
       <c r="U30" s="25"/>
     </row>
@@ -9775,7 +9775,7 @@
         <v>268</v>
       </c>
       <c r="S31" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="T31" s="31" t="s">
         <v>126</v>
@@ -9787,10 +9787,10 @@
         <v>115</v>
       </c>
       <c r="S32" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="T32" s="24" t="s">
         <v>233</v>
-      </c>
-      <c r="T32" s="24" t="s">
-        <v>234</v>
       </c>
       <c r="U32" s="25"/>
     </row>
@@ -9799,7 +9799,7 @@
         <v>50</v>
       </c>
       <c r="S33" s="29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T33" s="31" t="s">
         <v>84</v>
@@ -9811,7 +9811,7 @@
         <v>390</v>
       </c>
       <c r="S34" s="29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T34" s="24" t="s">
         <v>61</v>
@@ -9826,7 +9826,7 @@
         <v>44110</v>
       </c>
       <c r="T35" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="U35" s="25"/>
     </row>
@@ -9835,10 +9835,10 @@
         <v>200</v>
       </c>
       <c r="S36" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="T36" s="24" t="s">
         <v>237</v>
-      </c>
-      <c r="T36" s="24" t="s">
-        <v>238</v>
       </c>
       <c r="U36" s="25"/>
     </row>
@@ -9847,10 +9847,10 @@
         <v>94</v>
       </c>
       <c r="S37" s="29" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="T37" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="U37" s="25"/>
     </row>
@@ -10251,7 +10251,7 @@
         <v>43837</v>
       </c>
       <c r="T6" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U6" s="25"/>
     </row>
@@ -10298,7 +10298,7 @@
         <v>43897</v>
       </c>
       <c r="T7" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U7" s="25"/>
     </row>
@@ -10331,10 +10331,10 @@
         <v>100</v>
       </c>
       <c r="S8" s="29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T8" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U8" s="25"/>
     </row>
@@ -10415,7 +10415,7 @@
         <v>43897</v>
       </c>
       <c r="T10" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U10" s="25"/>
     </row>
@@ -10497,7 +10497,7 @@
         <v>43958</v>
       </c>
       <c r="T12" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U12" s="25"/>
     </row>
@@ -10556,7 +10556,7 @@
         <v>43958</v>
       </c>
       <c r="T14" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U14" s="25"/>
     </row>
@@ -10604,7 +10604,7 @@
         <v>44111</v>
       </c>
       <c r="T16" s="24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U16" s="25"/>
     </row>
@@ -10628,7 +10628,7 @@
         <v>44111</v>
       </c>
       <c r="T17" s="24" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="U17" s="25"/>
     </row>
@@ -10700,7 +10700,7 @@
         <v>44111</v>
       </c>
       <c r="T20" s="24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U20" s="25"/>
     </row>
@@ -10718,10 +10718,10 @@
         <v>130</v>
       </c>
       <c r="S21" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="T21" s="24" t="s">
         <v>245</v>
-      </c>
-      <c r="T21" s="24" t="s">
-        <v>246</v>
       </c>
       <c r="U21" s="25"/>
     </row>
@@ -10739,7 +10739,7 @@
         <v>333</v>
       </c>
       <c r="S22" s="29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T22" s="24" t="s">
         <v>61</v>
@@ -10760,10 +10760,10 @@
         <v>80</v>
       </c>
       <c r="S23" s="29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="T23" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U23" s="25"/>
     </row>
@@ -10781,10 +10781,10 @@
         <v>169</v>
       </c>
       <c r="S24" s="29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="T24" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U24" s="25"/>
     </row>
@@ -10802,7 +10802,7 @@
         <v>106</v>
       </c>
       <c r="S25" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T25" s="24" t="s">
         <v>84</v>
@@ -10823,7 +10823,7 @@
         <v>105</v>
       </c>
       <c r="S26" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T26" s="24" t="s">
         <v>59</v>
@@ -10844,7 +10844,7 @@
         <v>50</v>
       </c>
       <c r="S27" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T27" s="24" t="s">
         <v>84</v>
@@ -10865,7 +10865,7 @@
         <v>30</v>
       </c>
       <c r="S28" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T28" s="24" t="s">
         <v>59</v>
@@ -10886,7 +10886,7 @@
         <v>313</v>
       </c>
       <c r="S29" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="T29" s="24" t="s">
         <v>61</v>
@@ -10907,7 +10907,7 @@
         <v>47</v>
       </c>
       <c r="S30" s="29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="T30" s="31" t="s">
         <v>70</v>
@@ -10930,10 +10930,10 @@
         <v>114</v>
       </c>
       <c r="S31" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T31" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="U31" s="25"/>
     </row>
@@ -10942,10 +10942,10 @@
         <v>18</v>
       </c>
       <c r="S32" s="29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="T32" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U32" s="25"/>
     </row>
@@ -10954,7 +10954,7 @@
         <v>102</v>
       </c>
       <c r="S33" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T33" s="31" t="s">
         <v>84</v>
@@ -10966,7 +10966,7 @@
         <v>166</v>
       </c>
       <c r="S34" s="29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="T34" s="24" t="s">
         <v>84</v>
@@ -10978,10 +10978,10 @@
         <v>110</v>
       </c>
       <c r="S35" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T35" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U35" s="25"/>
     </row>
@@ -10990,7 +10990,7 @@
         <v>361</v>
       </c>
       <c r="S36" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T36" s="24" t="s">
         <v>61</v>
@@ -11002,10 +11002,10 @@
         <v>80</v>
       </c>
       <c r="S37" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="T37" s="24" t="s">
         <v>255</v>
-      </c>
-      <c r="T37" s="24" t="s">
-        <v>256</v>
       </c>
       <c r="U37" s="25"/>
     </row>
@@ -11014,7 +11014,7 @@
         <v>395</v>
       </c>
       <c r="S38" s="29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T38" s="24" t="s">
         <v>131</v>
@@ -11026,10 +11026,10 @@
         <v>82</v>
       </c>
       <c r="S39" s="29" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="T39" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U39" s="25"/>
     </row>
@@ -11038,10 +11038,10 @@
         <v>103</v>
       </c>
       <c r="S40" s="29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="T40" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U40" s="25"/>
     </row>
@@ -11050,10 +11050,10 @@
         <v>268</v>
       </c>
       <c r="S41" s="29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="T41" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="U41" s="25"/>
     </row>
@@ -11180,7 +11180,7 @@
   </sheetPr>
   <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -11364,7 +11364,7 @@
         <v>750</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="16">
@@ -11434,7 +11434,7 @@
         <v>43838</v>
       </c>
       <c r="T6" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U6" s="25"/>
     </row>
@@ -11481,7 +11481,7 @@
         <v>43838</v>
       </c>
       <c r="T7" s="24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="U7" s="25"/>
     </row>
@@ -11517,7 +11517,7 @@
         <v>43929</v>
       </c>
       <c r="T8" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="U8" s="25"/>
     </row>
@@ -11562,7 +11562,7 @@
         <v>43990</v>
       </c>
       <c r="T9" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U9" s="25"/>
     </row>
@@ -11598,7 +11598,7 @@
         <v>43990</v>
       </c>
       <c r="T10" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U10" s="25"/>
     </row>
@@ -11763,7 +11763,7 @@
         <v>44082</v>
       </c>
       <c r="T15" s="24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="U15" s="25"/>
     </row>
@@ -11787,7 +11787,7 @@
         <v>44051</v>
       </c>
       <c r="T16" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="U16" s="25"/>
     </row>
@@ -11835,7 +11835,7 @@
         <v>44143</v>
       </c>
       <c r="T18" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="U18" s="25"/>
     </row>
@@ -11904,7 +11904,7 @@
         <v>44143</v>
       </c>
       <c r="T21" s="24" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="U21" s="25"/>
     </row>
@@ -11925,7 +11925,7 @@
         <v>44143</v>
       </c>
       <c r="T22" s="24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U22" s="25"/>
     </row>
@@ -11964,7 +11964,7 @@
         <v>15</v>
       </c>
       <c r="S24" s="29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T24" s="24" t="s">
         <v>141</v>
@@ -11985,7 +11985,7 @@
         <v>17</v>
       </c>
       <c r="S25" s="29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T25" s="24" t="s">
         <v>59</v>
@@ -12006,7 +12006,7 @@
         <v>82</v>
       </c>
       <c r="S26" s="29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T26" s="24" t="s">
         <v>84</v>
@@ -12027,7 +12027,7 @@
         <v>31</v>
       </c>
       <c r="S27" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="T27" s="24" t="s">
         <v>70</v>
@@ -12048,7 +12048,7 @@
         <v>30</v>
       </c>
       <c r="S28" s="29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T28" s="24" t="s">
         <v>73</v>
@@ -12069,10 +12069,10 @@
         <v>184</v>
       </c>
       <c r="S29" s="35" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T29" s="24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="U29" s="25"/>
     </row>
@@ -12090,7 +12090,7 @@
         <v>169</v>
       </c>
       <c r="S30" s="29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="T30" s="31" t="s">
         <v>83</v>
@@ -12113,7 +12113,7 @@
         <v>132</v>
       </c>
       <c r="S31" s="29" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="T31" s="31" t="s">
         <v>84</v>
@@ -12125,7 +12125,7 @@
         <v>26</v>
       </c>
       <c r="S32" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="T32" s="24" t="s">
         <v>73</v>
@@ -12137,10 +12137,10 @@
         <v>73</v>
       </c>
       <c r="S33" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="T33" s="31" t="s">
         <v>270</v>
-      </c>
-      <c r="T33" s="31" t="s">
-        <v>271</v>
       </c>
       <c r="U33" s="25"/>
     </row>
@@ -12149,7 +12149,7 @@
         <v>50</v>
       </c>
       <c r="S34" s="29" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="T34" s="24" t="s">
         <v>73</v>
@@ -12161,7 +12161,7 @@
         <v>395</v>
       </c>
       <c r="S35" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="T35" s="24" t="s">
         <v>61</v>
@@ -12173,10 +12173,10 @@
         <v>90</v>
       </c>
       <c r="S36" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="T36" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="U36" s="25"/>
     </row>
@@ -12185,10 +12185,10 @@
         <v>191</v>
       </c>
       <c r="S37" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="T37" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U37" s="25"/>
     </row>
@@ -12197,7 +12197,7 @@
         <v>10</v>
       </c>
       <c r="S38" s="29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="T38" s="24" t="s">
         <v>61</v>
@@ -12209,7 +12209,7 @@
         <v>75</v>
       </c>
       <c r="S39" s="29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="T39" s="24" t="s">
         <v>84</v>
@@ -12221,7 +12221,7 @@
         <v>130</v>
       </c>
       <c r="S40" s="29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T40" s="24" t="s">
         <v>84</v>
@@ -12233,7 +12233,7 @@
         <v>64</v>
       </c>
       <c r="S41" s="29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T41" s="24" t="s">
         <v>59</v>

</xml_diff>